<commit_message>
Actualizada plantilla de entrada (Plantilla_Entrada_5W1H.xlsx)
</commit_message>
<xml_diff>
--- a/Plantilla_Entrada_5W1H.xlsx
+++ b/Plantilla_Entrada_5W1H.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NavaG\Downloads\5W1H\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B93843F-FCC1-4BEB-B9E8-1396B8716345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574A8678-332C-46E4-B372-A69FF24AA3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="738" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="949" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -22,8 +22,22 @@
     <sheet name="5_MarcaEjemplo_1" sheetId="7" r:id="rId7"/>
     <sheet name="5_MarcaEjemplo_2" sheetId="8" r:id="rId8"/>
     <sheet name="6_Categoria_XX" sheetId="9" r:id="rId9"/>
+    <sheet name="6_Categoria_1" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -905,8 +919,102 @@
 </comments>
 </file>
 
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>plantilla</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{8AA6A626-AFD6-4E6A-A9A2-829F06E610A0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Fecha (inicio de mes).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{3C212BA9-90DC-43A8-B5F5-9E5441C1BB68}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Volumen sell-in para esta categoría.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{15519773-B526-4C60-9129-76C79058574F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Volumen sell-in para esta categoría.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{8C00D3C2-D609-4D9C-87D4-1C6056597EAE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Volumen sell-in para esta categoría.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{C82E526B-FC37-482E-AE5A-69A1FF6065B7}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Volumen sell-in para esta categoría.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{CEC5ECD2-1848-46D5-B3BF-DBABF9EDD216}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Volumen sell-in para esta categoría.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
   <si>
     <t>Plantilla de Entrada 5W1H</t>
   </si>
@@ -1080,6 +1188,9 @@
   </si>
   <si>
     <t>  - `Y` solo se usa para subpreguntas (`3-1` tamaños, `3-2` marcas, `3-3` sabores, `5-1` regiones, `5-2` canales, etc.).</t>
+  </si>
+  <si>
+    <t>Total Marcas</t>
   </si>
 </sst>
 </file>
@@ -1511,7 +1622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
     </sheetView>
@@ -1684,6 +1795,526 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13302789-01E4-4A9A-A1E7-9BFEECAC6223}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>44927</v>
+      </c>
+      <c r="B2" s="14">
+        <v>2000000</v>
+      </c>
+      <c r="C2" s="14">
+        <v>615705.4</v>
+      </c>
+      <c r="D2" s="14">
+        <v>3078527</v>
+      </c>
+      <c r="E2" s="14">
+        <v>4197878</v>
+      </c>
+      <c r="F2" s="14">
+        <v>5336588</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>44958</v>
+      </c>
+      <c r="B3" s="14">
+        <v>2066351</v>
+      </c>
+      <c r="C3" s="14">
+        <v>635548.4</v>
+      </c>
+      <c r="D3" s="14">
+        <v>3177742</v>
+      </c>
+      <c r="E3" s="14">
+        <v>4313937</v>
+      </c>
+      <c r="F3" s="14">
+        <v>5448775</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>44986</v>
+      </c>
+      <c r="B4" s="14">
+        <v>2126939</v>
+      </c>
+      <c r="C4" s="14">
+        <v>652124</v>
+      </c>
+      <c r="D4" s="14">
+        <v>3260620</v>
+      </c>
+      <c r="E4" s="14">
+        <v>4400353</v>
+      </c>
+      <c r="F4" s="14">
+        <v>5518163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>45017</v>
+      </c>
+      <c r="B5" s="14">
+        <v>2176635</v>
+      </c>
+      <c r="C5" s="14">
+        <v>664253</v>
+      </c>
+      <c r="D5" s="14">
+        <v>3321265</v>
+      </c>
+      <c r="E5" s="14">
+        <v>4452531</v>
+      </c>
+      <c r="F5" s="14">
+        <v>5543719</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>45047</v>
+      </c>
+      <c r="B6" s="14">
+        <v>2211510</v>
+      </c>
+      <c r="C6" s="14">
+        <v>671246.20000000007</v>
+      </c>
+      <c r="D6" s="14">
+        <v>3356231</v>
+      </c>
+      <c r="E6" s="14">
+        <v>4469642</v>
+      </c>
+      <c r="F6" s="14">
+        <v>5529234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>45078</v>
+      </c>
+      <c r="B7" s="14">
+        <v>2229265</v>
+      </c>
+      <c r="C7" s="14">
+        <v>672979.60000000009</v>
+      </c>
+      <c r="D7" s="14">
+        <v>3364898</v>
+      </c>
+      <c r="E7" s="14">
+        <v>4454721</v>
+      </c>
+      <c r="F7" s="14">
+        <v>5482909</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>45108</v>
+      </c>
+      <c r="B8" s="14">
+        <v>2229488</v>
+      </c>
+      <c r="C8" s="14">
+        <v>669908.20000000007</v>
+      </c>
+      <c r="D8" s="14">
+        <v>3349541</v>
+      </c>
+      <c r="E8" s="14">
+        <v>4414327</v>
+      </c>
+      <c r="F8" s="14">
+        <v>5416448</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>45139</v>
+      </c>
+      <c r="B9" s="14">
+        <v>2213694</v>
+      </c>
+      <c r="C9" s="14">
+        <v>663015.80000000005</v>
+      </c>
+      <c r="D9" s="14">
+        <v>3315079</v>
+      </c>
+      <c r="E9" s="14">
+        <v>4357825</v>
+      </c>
+      <c r="F9" s="14">
+        <v>5343773</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>45170</v>
+      </c>
+      <c r="B10" s="14">
+        <v>2185164</v>
+      </c>
+      <c r="C10" s="14">
+        <v>653707</v>
+      </c>
+      <c r="D10" s="14">
+        <v>3268535</v>
+      </c>
+      <c r="E10" s="14">
+        <v>4296352</v>
+      </c>
+      <c r="F10" s="14">
+        <v>5279489</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <v>45200</v>
+      </c>
+      <c r="B11" s="14">
+        <v>2148579</v>
+      </c>
+      <c r="C11" s="14">
+        <v>643652.80000000005</v>
+      </c>
+      <c r="D11" s="14">
+        <v>3218264</v>
+      </c>
+      <c r="E11" s="14">
+        <v>4241591</v>
+      </c>
+      <c r="F11" s="14">
+        <v>5237279</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
+        <v>45231</v>
+      </c>
+      <c r="B12" s="14">
+        <v>2109509</v>
+      </c>
+      <c r="C12" s="14">
+        <v>634605.4</v>
+      </c>
+      <c r="D12" s="14">
+        <v>3173027</v>
+      </c>
+      <c r="E12" s="14">
+        <v>4204490</v>
+      </c>
+      <c r="F12" s="14">
+        <v>5228394</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
+        <v>45261</v>
+      </c>
+      <c r="B13" s="14">
+        <v>2073796</v>
+      </c>
+      <c r="C13" s="14">
+        <v>628206.80000000005</v>
+      </c>
+      <c r="D13" s="14">
+        <v>3141034</v>
+      </c>
+      <c r="E13" s="14">
+        <v>4194049</v>
+      </c>
+      <c r="F13" s="14">
+        <v>5260418</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>45292</v>
+      </c>
+      <c r="B14" s="14">
+        <v>2046912</v>
+      </c>
+      <c r="C14" s="14">
+        <v>625807.4</v>
+      </c>
+      <c r="D14" s="14">
+        <v>3129037</v>
+      </c>
+      <c r="E14" s="14">
+        <v>4216334</v>
+      </c>
+      <c r="F14" s="14">
+        <v>5336430</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
+        <v>45323</v>
+      </c>
+      <c r="B15" s="14">
+        <v>2033358</v>
+      </c>
+      <c r="C15" s="14">
+        <v>628316.80000000005</v>
+      </c>
+      <c r="D15" s="14">
+        <v>3141584</v>
+      </c>
+      <c r="E15" s="14">
+        <v>4273811</v>
+      </c>
+      <c r="F15" s="14">
+        <v>5454668</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
+        <v>45352</v>
+      </c>
+      <c r="B16" s="14">
+        <v>2036167</v>
+      </c>
+      <c r="C16" s="14">
+        <v>636105</v>
+      </c>
+      <c r="D16" s="14">
+        <v>3180525</v>
+      </c>
+      <c r="E16" s="14">
+        <v>4365068</v>
+      </c>
+      <c r="F16" s="14">
+        <v>5608721</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
+        <v>45383</v>
+      </c>
+      <c r="B17" s="14">
+        <v>2056572</v>
+      </c>
+      <c r="C17" s="14">
+        <v>648960.20000000007</v>
+      </c>
+      <c r="D17" s="14">
+        <v>3244801</v>
+      </c>
+      <c r="E17" s="14">
+        <v>4484977</v>
+      </c>
+      <c r="F17" s="14">
+        <v>5788234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
+        <v>45413</v>
+      </c>
+      <c r="B18" s="14">
+        <v>2093867</v>
+      </c>
+      <c r="C18" s="14">
+        <v>666113.20000000007</v>
+      </c>
+      <c r="D18" s="14">
+        <v>3330566</v>
+      </c>
+      <c r="E18" s="14">
+        <v>4625254</v>
+      </c>
+      <c r="F18" s="14">
+        <v>5980051</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
+        <v>45444</v>
+      </c>
+      <c r="B19" s="14">
+        <v>2145488</v>
+      </c>
+      <c r="C19" s="14">
+        <v>686321.4</v>
+      </c>
+      <c r="D19" s="14">
+        <v>3431607</v>
+      </c>
+      <c r="E19" s="14">
+        <v>4775374</v>
+      </c>
+      <c r="F19" s="14">
+        <v>6169660</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
+        <v>45474</v>
+      </c>
+      <c r="B20" s="14">
+        <v>2207294</v>
+      </c>
+      <c r="C20" s="14">
+        <v>708006</v>
+      </c>
+      <c r="D20" s="14">
+        <v>3540030</v>
+      </c>
+      <c r="E20" s="14">
+        <v>4923728</v>
+      </c>
+      <c r="F20" s="14">
+        <v>6342795</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
+        <v>45505</v>
+      </c>
+      <c r="B21" s="14">
+        <v>2274020</v>
+      </c>
+      <c r="C21" s="14">
+        <v>729426</v>
+      </c>
+      <c r="D21" s="14">
+        <v>3647130</v>
+      </c>
+      <c r="E21" s="14">
+        <v>5058902</v>
+      </c>
+      <c r="F21" s="14">
+        <v>6486999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
+        <v>45536</v>
+      </c>
+      <c r="B22" s="14">
+        <v>2339864</v>
+      </c>
+      <c r="C22" s="14">
+        <v>748868.60000000009</v>
+      </c>
+      <c r="D22" s="14">
+        <v>3744343</v>
+      </c>
+      <c r="E22" s="14">
+        <v>5170932</v>
+      </c>
+      <c r="F22" s="14">
+        <v>6593003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="13">
+        <v>45566</v>
+      </c>
+      <c r="B23" s="14">
+        <v>2399118</v>
+      </c>
+      <c r="C23" s="14">
+        <v>764839.8</v>
+      </c>
+      <c r="D23" s="14">
+        <v>3824199</v>
+      </c>
+      <c r="E23" s="14">
+        <v>5252402</v>
+      </c>
+      <c r="F23" s="14">
+        <v>6655743</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="13">
+        <v>45597</v>
+      </c>
+      <c r="B24" s="14">
+        <v>2446799</v>
+      </c>
+      <c r="C24" s="14">
+        <v>776227</v>
+      </c>
+      <c r="D24" s="14">
+        <v>3881135</v>
+      </c>
+      <c r="E24" s="14">
+        <v>5299261</v>
+      </c>
+      <c r="F24" s="14">
+        <v>6674918</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="13">
+        <v>45627</v>
+      </c>
+      <c r="B25" s="14">
+        <v>2479201</v>
+      </c>
+      <c r="C25" s="14">
+        <v>782422.60000000009</v>
+      </c>
+      <c r="D25" s="14">
+        <v>3912113</v>
+      </c>
+      <c r="E25" s="14">
+        <v>5311267</v>
+      </c>
+      <c r="F25" s="14">
+        <v>6655020</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Mejoras en índice de precio y opciones de estilo en gráficas
- Añade parámetros color_collector, color_overrides y linestyle_overrides a line_graf; aplica overrides, preserva mapping y recopila colores de series.
- Evita anotar la serie 'Total' en las anotaciones top y permite overrides de estilo/linestyle por serie.
- Modifica prepare_price_index_dataframe para devolver también el DataFrame original, calcular ratios en % y manejar NaN/inf de forma robusta.
- Añade graf_price_index_table para generar una tabla PNG con promedios (12m) y la integra en build_price_index_slide; calcula promedios relativos al Total cuando procede y ajusta layout/escala y posición.
- Ajusta altura del gráfico en la slide, pasa price_original_df en los llamadores y mejora el posicionamiento/colores (incluyendo estilo/color por defecto para 'Total').
- Actualiza plantilla de entrada (Plantilla_Entrada_5W1H.xlsx).
</commit_message>
<xml_diff>
--- a/Plantilla_Entrada_5W1H.xlsx
+++ b/Plantilla_Entrada_5W1H.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NavaG\Downloads\5W1H\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574A8678-332C-46E4-B372-A69FF24AA3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14307A5D-288F-4B9C-A661-5803B548EF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="949" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25380" yWindow="21480" windowWidth="20730" windowHeight="11040" tabRatio="949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -1014,7 +1014,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
   <si>
     <t>Plantilla de Entrada 5W1H</t>
   </si>
@@ -1190,14 +1190,17 @@
     <t>  - `Y` solo se usa para subpreguntas (`3-1` tamaños, `3-2` marcas, `3-3` sabores, `5-1` regiones, `5-2` canales, etc.).</t>
   </si>
   <si>
-    <t>Total Marcas</t>
+    <t>Total Categoria</t>
+  </si>
+  <si>
+    <t>  - `6-1`: Competencia, Precio Indexado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1228,8 +1231,15 @@
       <color rgb="FF1F1F1F"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1261,6 +1271,12 @@
         <fgColor rgb="FFC6E0B4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1283,7 +1299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1318,6 +1334,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1620,11 +1639,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,6 +1809,11 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1802,9 +1826,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13302789-01E4-4A9A-A1E7-9BFEECAC6223}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1816,7 +1840,7 @@
       <c r="A1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="18" t="s">
         <v>58</v>
       </c>
       <c r="C1" s="12" t="s">

</xml_diff>

<commit_message>
Actualizada la plantilla de entrada 'Plantilla_Entrada_5W1H.xlsx' para reflejar cambios en los datos.
</commit_message>
<xml_diff>
--- a/Plantilla_Entrada_5W1H.xlsx
+++ b/Plantilla_Entrada_5W1H.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NavaG\Downloads\5W1H\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14307A5D-288F-4B9C-A661-5803B548EF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFEC3EB-7915-4BD5-A010-BCAF3B92A462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25380" yWindow="21480" windowWidth="20730" windowHeight="11040" tabRatio="949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="34605" windowHeight="20985" tabRatio="949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -1014,7 +1014,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
   <si>
     <t>Plantilla de Entrada 5W1H</t>
   </si>
@@ -1151,9 +1151,6 @@
     <t>  - `1`: Cuando? (grafico MAT).</t>
   </si>
   <si>
-    <t>  - `2`: Por que? (arbol cargado fuera del script).</t>
-  </si>
-  <si>
     <t>  - `3-1`: Que? Tamanos.</t>
   </si>
   <si>
@@ -1194,6 +1191,12 @@
   </si>
   <si>
     <t>  - `6-1`: Competencia, Precio Indexado</t>
+  </si>
+  <si>
+    <t>U/L/K/T/R/M</t>
+  </si>
+  <si>
+    <t>  - `2-Unidad`: Por que? (arbol - datos MAT).</t>
   </si>
 </sst>
 </file>
@@ -1643,7 +1646,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,93 +1735,97 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1841,7 +1848,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Actualización de la plantilla de entrada de Excel para mejorar la estructura de datos.
</commit_message>
<xml_diff>
--- a/Plantilla_Entrada_5W1H.xlsx
+++ b/Plantilla_Entrada_5W1H.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NavaG\Downloads\5W1H\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE66887-A0F9-4105-9AED-D0C9BE829A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997E2638-F046-46C3-B75B-7DF601E93E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="949" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="10545" tabRatio="949" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -1298,23 +1298,27 @@
       <sz val="16"/>
       <color rgb="FF1F4E79"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF1F1F1F"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="13"/>
       <color rgb="FF1F1F1F"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF1F1F1F"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1384,7 +1388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1422,7 +1426,6 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3178,7 +3181,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:C17"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3258,112 +3261,112 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8">
         <v>100</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8">
         <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9">
         <v>7.3</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9">
         <v>14.1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10">
         <v>100</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10">
         <v>193.6</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11">
         <v>0.54</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11">
         <v>0.43</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="A12" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12">
         <v>28.44</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12">
         <v>37.47</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="A13" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13">
         <v>4.2300000000000004</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13">
         <v>5.57</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14">
         <v>0.26</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14">
         <v>0.25</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="19">
+      <c r="B15">
         <v>14.04</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15">
         <v>21.88</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="A16" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B16">
         <v>2.09</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16">
         <v>3.25</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="A17" t="s">
         <v>79</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17">
         <v>2</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17">
         <v>1.7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualiza el archivo Plantilla_Entrada_5W1H.xlsx para mejorar la estructura y funcionalidad de los datos.
</commit_message>
<xml_diff>
--- a/Plantilla_Entrada_5W1H.xlsx
+++ b/Plantilla_Entrada_5W1H.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NavaG\Downloads\5W1H\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997E2638-F046-46C3-B75B-7DF601E93E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C60F9BA-7A02-4AAE-89D0-CA315DFFB737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="10545" tabRatio="949" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="949" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="5_MarcaEjemplo_2" sheetId="8" r:id="rId9"/>
     <sheet name="6_Categoria_XX" sheetId="9" r:id="rId10"/>
     <sheet name="6_Categoria_1" sheetId="10" r:id="rId11"/>
+    <sheet name="7_Categoria_Canal" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1015,7 +1016,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="98">
   <si>
     <t>Plantilla de Entrada 5W1H</t>
   </si>
@@ -1279,6 +1280,36 @@
   </si>
   <si>
     <t>BUYERS</t>
+  </si>
+  <si>
+    <t>Measures = Weighted R_VOL1 Vert %</t>
+  </si>
+  <si>
+    <t>_PERIODS = MAT Jun-25\Total _PERIODS</t>
+  </si>
+  <si>
+    <t>crch54kw - table - 05/12/2025 05:47:34 p. m.</t>
+  </si>
+  <si>
+    <t>T. Quesos Blancos+ Fundidos</t>
+  </si>
+  <si>
+    <t>La Serenísima Clásico</t>
+  </si>
+  <si>
+    <t>Casancrem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total BFPCH  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Modern Trade  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Traditional Trade  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Other Channels  </t>
   </si>
 </sst>
 </file>
@@ -2880,6 +2911,101 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F55B0E1-EB16-4274-B21C-3BAC2F1EFA62}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="C5">
+        <v>72.2</v>
+      </c>
+      <c r="D5">
+        <v>75.900000000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6">
+        <v>24.3</v>
+      </c>
+      <c r="C6">
+        <v>27.1</v>
+      </c>
+      <c r="D6">
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C7">
+        <v>0.7</v>
+      </c>
+      <c r="D7">
+        <v>0.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C25"/>
@@ -3180,7 +3306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C569621-BA5C-4664-99F2-184EDE95915C}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Corrige mensajes de advertencia para incluir comillas en los encabezados de "Compras" y "Ventas" en la función split_compras_ventas.
</commit_message>
<xml_diff>
--- a/Plantilla_Entrada_5W1H.xlsx
+++ b/Plantilla_Entrada_5W1H.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NavaG\Downloads\5W1H\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C60F9BA-7A02-4AAE-89D0-CA315DFFB737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AD167F-A003-446F-AF3C-D8D6E78E5DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="949" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -1016,7 +1016,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="100">
   <si>
     <t>Plantilla de Entrada 5W1H</t>
   </si>
@@ -1310,6 +1310,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Other Channels  </t>
+  </si>
+  <si>
+    <t>  - `7-Perfil`: Distribucion de perfiles MAT categoria</t>
+  </si>
+  <si>
+    <t>Canal/ Region/ NSE/ Pais/ Gramaje</t>
   </si>
 </sst>
 </file>
@@ -1759,11 +1765,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1920,23 +1926,31 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2915,7 +2929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F55B0E1-EB16-4274-B21C-3BAC2F1EFA62}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ajusta propiedades de texto en la tabla de PowerPoint y mejora la claridad de los títulos en los intervalos de confianza. Se complemento la plantilla de entrada para poder visualiza bien la informacion esperada de entrada
</commit_message>
<xml_diff>
--- a/Plantilla_Entrada_5W1H.xlsx
+++ b/Plantilla_Entrada_5W1H.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NavaG\Downloads\5W1H\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AD167F-A003-446F-AF3C-D8D6E78E5DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22486E58-B2C3-40B0-ABFE-BBA91A767CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="949" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="6_Categoria_XX" sheetId="9" r:id="rId10"/>
     <sheet name="6_Categoria_1" sheetId="10" r:id="rId11"/>
     <sheet name="7_Categoria_Canal" sheetId="12" r:id="rId12"/>
+    <sheet name="8_Categoria" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1016,7 +1017,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="267">
   <si>
     <t>Plantilla de Entrada 5W1H</t>
   </si>
@@ -1316,6 +1317,507 @@
   </si>
   <si>
     <t>Canal/ Region/ NSE/ Pais/ Gramaje</t>
+  </si>
+  <si>
+    <t>  - `8-Categoria`:Intervalos de confianza</t>
+  </si>
+  <si>
+    <t>brea93bi - table - 10/12/2025 04:28:51 p. m.</t>
+  </si>
+  <si>
+    <t>MAT Aug-24</t>
+  </si>
+  <si>
+    <t>MAT Aug-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bimbo  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Jan-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Weighted R_VOL1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Feb-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Weighted R_VOL1 Vert %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Mar-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Weighted VOL1_P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Apr-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Weighted VAL_LC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   May-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Weighted VAL_LC Vert %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Jun-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Weighted VAL_US</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Jul-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Weighted VAL_US Vert %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Aug-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Weighted PENET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Sep-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Weighted PENET Vert %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Oct-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Weighted VO1_BUY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Nov-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Weighted VALC_BUY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Dec-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Weighted VAUS_BUY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Jan-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Weighted VO1_DAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Feb-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Weighted VALC_DAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Mar-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Weighted VAUS_DAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Apr-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Weighted FREQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   May-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Weighted PM1_LC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Jun-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Weighted PM1_US</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Jul-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Weighted HHOLDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Aug-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Weighted HHOLDS Vert %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Sep-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Weighted BUYERS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Oct-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Weighted BUYERS Vert %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Nov-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   HHOLDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Dec-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   BUYERS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Jan-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Feb-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Grile  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Mar-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Weighted R_VOL1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Apr-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Weighted R_VOL1 Vert %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   May-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Weighted VOL1_P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Jun-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Weighted VAL_LC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Jul-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Weighted VAL_LC Vert %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Aug-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Weighted VAL_US</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Sep-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Weighted VAL_US Vert %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Oct-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Weighted PENET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Nov-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Weighted PENET Vert %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Dec-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Weighted VO1_BUY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Jan-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Weighted VALC_BUY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Feb-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Weighted VAUS_BUY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Mar-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Weighted VO1_DAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Apr-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Weighted VALC_DAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   May-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Weighted VAUS_DAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Jun-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Weighted FREQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Jul-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Weighted PM1_LC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Aug-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Weighted PM1_US</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Sep-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Weighted HHOLDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Oct-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Weighted HHOLDS Vert %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Nov-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Weighted BUYERS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Dec-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Weighted BUYERS Vert %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Jan-25  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    HHOLDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Feb-25  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    BUYERS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Mar-25  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Apr-25  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Bimbo  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   May-25  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Jun-25  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Jul-25  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Aug-25  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Jan-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Feb-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Mar-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Apr-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    May-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Jun-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Jul-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Aug-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Sep-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Oct-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Nov-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Dec-21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Jan-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Feb-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Mar-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Apr-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    May-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Jun-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Jul-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Aug-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Sep-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Oct-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Nov-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Dec-22  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Jan-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Feb-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Mar-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Apr-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    May-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Jun-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Jul-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Aug-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Sep-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Oct-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Nov-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Dec-23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Jan-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Feb-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Mar-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Apr-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    May-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Jun-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Jul-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Aug-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Sep-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Oct-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Nov-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Dec-24  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Jan-25  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Feb-25  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Mar-25  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Apr-25  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    May-25  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Jun-25  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Jul-25  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Aug-25  </t>
   </si>
 </sst>
 </file>
@@ -1365,7 +1867,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1403,6 +1905,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1425,7 +1933,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1463,6 +1971,8 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1478,6 +1988,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>595842</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>3734</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FC138FC-89A9-4AE5-9599-27BA988EB43D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12025842" y="0"/>
+          <a:ext cx="5509684" cy="3813734"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>295276</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>470960</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>106164</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58B2EC21-404B-45ED-8DDA-0700323E515E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6391276" y="0"/>
+          <a:ext cx="5509684" cy="2582664"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1765,9 +2368,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="6" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
@@ -1951,6 +2554,11 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>52</v>
       </c>
     </row>
@@ -3020,6 +3628,2566 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A3A67E-8AC6-4000-96DE-0ABA21917A59}">
+  <dimension ref="A1:G174"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="19"/>
+      <c r="E1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3">
+        <v>52.5</v>
+      </c>
+      <c r="C3">
+        <v>973</v>
+      </c>
+      <c r="E3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3">
+        <v>10944760</v>
+      </c>
+      <c r="G3">
+        <v>10923380</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4">
+        <v>51.1</v>
+      </c>
+      <c r="C4">
+        <v>961</v>
+      </c>
+      <c r="E4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5">
+        <v>52.6</v>
+      </c>
+      <c r="C5">
+        <v>998</v>
+      </c>
+      <c r="E5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F5">
+        <v>10945</v>
+      </c>
+      <c r="G5">
+        <v>10923</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6">
+        <v>52.9</v>
+      </c>
+      <c r="C6">
+        <v>988</v>
+      </c>
+      <c r="E6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6">
+        <v>48240360</v>
+      </c>
+      <c r="G6">
+        <v>47738220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7">
+        <v>53.6</v>
+      </c>
+      <c r="C7">
+        <v>1042</v>
+      </c>
+      <c r="E7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8">
+        <v>51.5</v>
+      </c>
+      <c r="C8">
+        <v>958</v>
+      </c>
+      <c r="E8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F8">
+        <v>48240360</v>
+      </c>
+      <c r="G8">
+        <v>47738220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9">
+        <v>50.7</v>
+      </c>
+      <c r="C9">
+        <v>957</v>
+      </c>
+      <c r="E9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
+      </c>
+      <c r="G9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10">
+        <v>48.5</v>
+      </c>
+      <c r="C10">
+        <v>921</v>
+      </c>
+      <c r="E10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F10">
+        <v>86.3</v>
+      </c>
+      <c r="G10">
+        <v>89.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11">
+        <v>45.2</v>
+      </c>
+      <c r="C11">
+        <v>846</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12">
+        <v>50.5</v>
+      </c>
+      <c r="C12">
+        <v>926</v>
+      </c>
+      <c r="E12" t="s">
+        <v>124</v>
+      </c>
+      <c r="F12">
+        <v>3.64</v>
+      </c>
+      <c r="G12">
+        <v>3.42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13">
+        <v>48.1</v>
+      </c>
+      <c r="C13">
+        <v>858</v>
+      </c>
+      <c r="E13" t="s">
+        <v>126</v>
+      </c>
+      <c r="F13">
+        <v>16.059999999999999</v>
+      </c>
+      <c r="G13">
+        <v>14.95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14">
+        <v>51.6</v>
+      </c>
+      <c r="C14">
+        <v>941</v>
+      </c>
+      <c r="E14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F14">
+        <v>16.059999999999999</v>
+      </c>
+      <c r="G14">
+        <v>14.95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15">
+        <v>51.1</v>
+      </c>
+      <c r="C15">
+        <v>923</v>
+      </c>
+      <c r="E15" t="s">
+        <v>130</v>
+      </c>
+      <c r="F15">
+        <v>0.5</v>
+      </c>
+      <c r="G15">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16">
+        <v>48.6</v>
+      </c>
+      <c r="C16">
+        <v>891</v>
+      </c>
+      <c r="E16" t="s">
+        <v>132</v>
+      </c>
+      <c r="F16">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G16">
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17">
+        <v>53.5</v>
+      </c>
+      <c r="C17">
+        <v>958</v>
+      </c>
+      <c r="E17" t="s">
+        <v>134</v>
+      </c>
+      <c r="F17">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G17">
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18">
+        <v>48.2</v>
+      </c>
+      <c r="C18">
+        <v>856</v>
+      </c>
+      <c r="E18" t="s">
+        <v>136</v>
+      </c>
+      <c r="F18">
+        <v>7.3</v>
+      </c>
+      <c r="G18">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19">
+        <v>48.2</v>
+      </c>
+      <c r="C19">
+        <v>865</v>
+      </c>
+      <c r="E19" t="s">
+        <v>138</v>
+      </c>
+      <c r="F19">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="G19">
+        <v>4.7300000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20">
+        <v>45.8</v>
+      </c>
+      <c r="C20">
+        <v>814</v>
+      </c>
+      <c r="E20" t="s">
+        <v>140</v>
+      </c>
+      <c r="F20">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="G20">
+        <v>4.7300000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B21">
+        <v>44.1</v>
+      </c>
+      <c r="C21">
+        <v>809</v>
+      </c>
+      <c r="E21" t="s">
+        <v>142</v>
+      </c>
+      <c r="F21">
+        <v>3483019</v>
+      </c>
+      <c r="G21">
+        <v>3576470</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>143</v>
+      </c>
+      <c r="B22">
+        <v>42.7</v>
+      </c>
+      <c r="C22">
+        <v>774</v>
+      </c>
+      <c r="E22" t="s">
+        <v>144</v>
+      </c>
+      <c r="F22">
+        <v>100</v>
+      </c>
+      <c r="G22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>145</v>
+      </c>
+      <c r="B23">
+        <v>41.4</v>
+      </c>
+      <c r="C23">
+        <v>746</v>
+      </c>
+      <c r="E23" t="s">
+        <v>146</v>
+      </c>
+      <c r="F23">
+        <v>3004475</v>
+      </c>
+      <c r="G23">
+        <v>3192965</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>147</v>
+      </c>
+      <c r="B24">
+        <v>42.5</v>
+      </c>
+      <c r="C24">
+        <v>766</v>
+      </c>
+      <c r="E24" t="s">
+        <v>148</v>
+      </c>
+      <c r="F24">
+        <v>100</v>
+      </c>
+      <c r="G24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>149</v>
+      </c>
+      <c r="B25">
+        <v>42.9</v>
+      </c>
+      <c r="C25">
+        <v>753</v>
+      </c>
+      <c r="E25" t="s">
+        <v>150</v>
+      </c>
+      <c r="F25">
+        <v>4704</v>
+      </c>
+      <c r="G25">
+        <v>3728</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26">
+        <v>41.1</v>
+      </c>
+      <c r="C26">
+        <v>743</v>
+      </c>
+      <c r="E26" t="s">
+        <v>152</v>
+      </c>
+      <c r="F26">
+        <v>3253</v>
+      </c>
+      <c r="G26">
+        <v>3026</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>153</v>
+      </c>
+      <c r="B27">
+        <v>37.4</v>
+      </c>
+      <c r="C27">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>154</v>
+      </c>
+      <c r="B28">
+        <v>39.5</v>
+      </c>
+      <c r="C28">
+        <v>689</v>
+      </c>
+      <c r="E28" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>156</v>
+      </c>
+      <c r="B29">
+        <v>40.6</v>
+      </c>
+      <c r="C29">
+        <v>715</v>
+      </c>
+      <c r="E29" t="s">
+        <v>157</v>
+      </c>
+      <c r="F29">
+        <v>591438</v>
+      </c>
+      <c r="G29">
+        <v>550419</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>158</v>
+      </c>
+      <c r="B30">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="C30">
+        <v>673</v>
+      </c>
+      <c r="E30" t="s">
+        <v>159</v>
+      </c>
+      <c r="F30">
+        <v>5.4</v>
+      </c>
+      <c r="G30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>160</v>
+      </c>
+      <c r="B31">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="C31">
+        <v>719</v>
+      </c>
+      <c r="E31" t="s">
+        <v>161</v>
+      </c>
+      <c r="F31">
+        <v>591</v>
+      </c>
+      <c r="G31">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>162</v>
+      </c>
+      <c r="B32">
+        <v>40.1</v>
+      </c>
+      <c r="C32">
+        <v>665</v>
+      </c>
+      <c r="E32" t="s">
+        <v>163</v>
+      </c>
+      <c r="F32">
+        <v>5927047</v>
+      </c>
+      <c r="G32">
+        <v>5826820</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>164</v>
+      </c>
+      <c r="B33">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="C33">
+        <v>1014</v>
+      </c>
+      <c r="E33" t="s">
+        <v>165</v>
+      </c>
+      <c r="F33">
+        <v>12.3</v>
+      </c>
+      <c r="G33">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>166</v>
+      </c>
+      <c r="B34">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="C34">
+        <v>947</v>
+      </c>
+      <c r="E34" t="s">
+        <v>167</v>
+      </c>
+      <c r="F34">
+        <v>5927047</v>
+      </c>
+      <c r="G34">
+        <v>5826820</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>168</v>
+      </c>
+      <c r="B35">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="C35">
+        <v>1013</v>
+      </c>
+      <c r="E35" t="s">
+        <v>169</v>
+      </c>
+      <c r="F35">
+        <v>12.3</v>
+      </c>
+      <c r="G35">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>170</v>
+      </c>
+      <c r="B36">
+        <v>37.1</v>
+      </c>
+      <c r="C36">
+        <v>959</v>
+      </c>
+      <c r="E36" t="s">
+        <v>171</v>
+      </c>
+      <c r="F36">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="G36">
+        <v>39.1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>172</v>
+      </c>
+      <c r="B37">
+        <v>37.1</v>
+      </c>
+      <c r="C37">
+        <v>966</v>
+      </c>
+      <c r="E37" t="s">
+        <v>173</v>
+      </c>
+      <c r="F37">
+        <v>40.4</v>
+      </c>
+      <c r="G37">
+        <v>43.8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>174</v>
+      </c>
+      <c r="B38">
+        <v>36.6</v>
+      </c>
+      <c r="C38">
+        <v>987</v>
+      </c>
+      <c r="E38" t="s">
+        <v>175</v>
+      </c>
+      <c r="F38">
+        <v>0.49</v>
+      </c>
+      <c r="G38">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>176</v>
+      </c>
+      <c r="B39">
+        <v>38.1</v>
+      </c>
+      <c r="C39">
+        <v>967</v>
+      </c>
+      <c r="E39" t="s">
+        <v>177</v>
+      </c>
+      <c r="F39">
+        <v>4.88</v>
+      </c>
+      <c r="G39">
+        <v>4.16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>178</v>
+      </c>
+      <c r="B40">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="C40">
+        <v>927</v>
+      </c>
+      <c r="E40" t="s">
+        <v>179</v>
+      </c>
+      <c r="F40">
+        <v>4.88</v>
+      </c>
+      <c r="G40">
+        <v>4.16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>180</v>
+      </c>
+      <c r="B41">
+        <v>36.5</v>
+      </c>
+      <c r="C41">
+        <v>969</v>
+      </c>
+      <c r="E41" t="s">
+        <v>181</v>
+      </c>
+      <c r="F41">
+        <v>0.16</v>
+      </c>
+      <c r="G41">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>182</v>
+      </c>
+      <c r="B42">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="C42">
+        <v>940</v>
+      </c>
+      <c r="E42" t="s">
+        <v>183</v>
+      </c>
+      <c r="F42">
+        <v>1.61</v>
+      </c>
+      <c r="G42">
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>184</v>
+      </c>
+      <c r="B43">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="C43">
+        <v>1056</v>
+      </c>
+      <c r="E43" t="s">
+        <v>185</v>
+      </c>
+      <c r="F43">
+        <v>1.61</v>
+      </c>
+      <c r="G43">
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>186</v>
+      </c>
+      <c r="B44">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="C44">
+        <v>1016</v>
+      </c>
+      <c r="E44" t="s">
+        <v>187</v>
+      </c>
+      <c r="F44">
+        <v>3</v>
+      </c>
+      <c r="G44">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>188</v>
+      </c>
+      <c r="B45">
+        <v>31.6</v>
+      </c>
+      <c r="C45">
+        <v>910</v>
+      </c>
+      <c r="E45" t="s">
+        <v>189</v>
+      </c>
+      <c r="F45">
+        <v>11.18</v>
+      </c>
+      <c r="G45">
+        <v>11.57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>190</v>
+      </c>
+      <c r="B46">
+        <v>32.5</v>
+      </c>
+      <c r="C46">
+        <v>883</v>
+      </c>
+      <c r="E46" t="s">
+        <v>191</v>
+      </c>
+      <c r="F46">
+        <v>11.18</v>
+      </c>
+      <c r="G46">
+        <v>11.57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>192</v>
+      </c>
+      <c r="B47">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="C47">
+        <v>943</v>
+      </c>
+      <c r="E47" t="s">
+        <v>193</v>
+      </c>
+      <c r="F47">
+        <v>3483019</v>
+      </c>
+      <c r="G47">
+        <v>3576470</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>194</v>
+      </c>
+      <c r="B48">
+        <v>32</v>
+      </c>
+      <c r="C48">
+        <v>918</v>
+      </c>
+      <c r="E48" t="s">
+        <v>195</v>
+      </c>
+      <c r="F48">
+        <v>100</v>
+      </c>
+      <c r="G48">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>196</v>
+      </c>
+      <c r="B49">
+        <v>34</v>
+      </c>
+      <c r="C49">
+        <v>900</v>
+      </c>
+      <c r="E49" t="s">
+        <v>197</v>
+      </c>
+      <c r="F49">
+        <v>1213634</v>
+      </c>
+      <c r="G49">
+        <v>1399966</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>198</v>
+      </c>
+      <c r="B50">
+        <v>30.3</v>
+      </c>
+      <c r="C50">
+        <v>886</v>
+      </c>
+      <c r="E50" t="s">
+        <v>199</v>
+      </c>
+      <c r="F50">
+        <v>40.4</v>
+      </c>
+      <c r="G50">
+        <v>43.8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>200</v>
+      </c>
+      <c r="B51">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="C51">
+        <v>920</v>
+      </c>
+      <c r="E51" t="s">
+        <v>201</v>
+      </c>
+      <c r="F51">
+        <v>4704</v>
+      </c>
+      <c r="G51">
+        <v>3728</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>202</v>
+      </c>
+      <c r="B52">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="C52">
+        <v>965</v>
+      </c>
+      <c r="E52" t="s">
+        <v>203</v>
+      </c>
+      <c r="F52">
+        <v>1132</v>
+      </c>
+      <c r="G52">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>204</v>
+      </c>
+      <c r="B53">
+        <v>35.9</v>
+      </c>
+      <c r="C53">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>205</v>
+      </c>
+      <c r="B54">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="C54">
+        <v>1001</v>
+      </c>
+      <c r="E54" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>207</v>
+      </c>
+      <c r="B55">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="C55">
+        <v>1012</v>
+      </c>
+      <c r="E55" t="s">
+        <v>157</v>
+      </c>
+      <c r="F55">
+        <v>2842228</v>
+      </c>
+      <c r="G55">
+        <v>2776101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>208</v>
+      </c>
+      <c r="B56">
+        <v>34.9</v>
+      </c>
+      <c r="C56">
+        <v>975</v>
+      </c>
+      <c r="E56" t="s">
+        <v>159</v>
+      </c>
+      <c r="F56">
+        <v>26</v>
+      </c>
+      <c r="G56">
+        <v>25.4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>209</v>
+      </c>
+      <c r="B57">
+        <v>31.7</v>
+      </c>
+      <c r="C57">
+        <v>1006</v>
+      </c>
+      <c r="E57" t="s">
+        <v>161</v>
+      </c>
+      <c r="F57">
+        <v>2842</v>
+      </c>
+      <c r="G57">
+        <v>2776</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>210</v>
+      </c>
+      <c r="B58">
+        <v>35.5</v>
+      </c>
+      <c r="C58">
+        <v>999</v>
+      </c>
+      <c r="E58" t="s">
+        <v>163</v>
+      </c>
+      <c r="F58">
+        <v>15197020</v>
+      </c>
+      <c r="G58">
+        <v>14607810</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
+        <v>165</v>
+      </c>
+      <c r="F59">
+        <v>31.5</v>
+      </c>
+      <c r="G59">
+        <v>30.6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>155</v>
+      </c>
+      <c r="E60" t="s">
+        <v>167</v>
+      </c>
+      <c r="F60">
+        <v>15197020</v>
+      </c>
+      <c r="G60">
+        <v>14607810</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>211</v>
+      </c>
+      <c r="B61">
+        <v>11.2</v>
+      </c>
+      <c r="C61">
+        <v>274</v>
+      </c>
+      <c r="E61" t="s">
+        <v>169</v>
+      </c>
+      <c r="F61">
+        <v>31.5</v>
+      </c>
+      <c r="G61">
+        <v>30.6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>212</v>
+      </c>
+      <c r="B62">
+        <v>12.2</v>
+      </c>
+      <c r="C62">
+        <v>274</v>
+      </c>
+      <c r="E62" t="s">
+        <v>171</v>
+      </c>
+      <c r="F62">
+        <v>54.6</v>
+      </c>
+      <c r="G62">
+        <v>58.4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>213</v>
+      </c>
+      <c r="B63">
+        <v>13.2</v>
+      </c>
+      <c r="C63">
+        <v>302</v>
+      </c>
+      <c r="E63" t="s">
+        <v>173</v>
+      </c>
+      <c r="F63">
+        <v>63.3</v>
+      </c>
+      <c r="G63">
+        <v>65.400000000000006</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>214</v>
+      </c>
+      <c r="B64">
+        <v>12</v>
+      </c>
+      <c r="C64">
+        <v>305</v>
+      </c>
+      <c r="E64" t="s">
+        <v>175</v>
+      </c>
+      <c r="F64">
+        <v>1.49</v>
+      </c>
+      <c r="G64">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>215</v>
+      </c>
+      <c r="B65">
+        <v>12.3</v>
+      </c>
+      <c r="C65">
+        <v>300</v>
+      </c>
+      <c r="E65" t="s">
+        <v>177</v>
+      </c>
+      <c r="F65">
+        <v>7.99</v>
+      </c>
+      <c r="G65">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>216</v>
+      </c>
+      <c r="B66">
+        <v>10.4</v>
+      </c>
+      <c r="C66">
+        <v>247</v>
+      </c>
+      <c r="E66" t="s">
+        <v>179</v>
+      </c>
+      <c r="F66">
+        <v>7.99</v>
+      </c>
+      <c r="G66">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>217</v>
+      </c>
+      <c r="B67">
+        <v>10.1</v>
+      </c>
+      <c r="C67">
+        <v>256</v>
+      </c>
+      <c r="E67" t="s">
+        <v>181</v>
+      </c>
+      <c r="F67">
+        <v>0.42</v>
+      </c>
+      <c r="G67">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>218</v>
+      </c>
+      <c r="B68">
+        <v>10.6</v>
+      </c>
+      <c r="C68">
+        <v>242</v>
+      </c>
+      <c r="E68" t="s">
+        <v>183</v>
+      </c>
+      <c r="F68">
+        <v>2.25</v>
+      </c>
+      <c r="G68">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>219</v>
+      </c>
+      <c r="B69">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="C69">
+        <v>222</v>
+      </c>
+      <c r="E69" t="s">
+        <v>185</v>
+      </c>
+      <c r="F69">
+        <v>2.25</v>
+      </c>
+      <c r="G69">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>220</v>
+      </c>
+      <c r="B70">
+        <v>11.5</v>
+      </c>
+      <c r="C70">
+        <v>249</v>
+      </c>
+      <c r="E70" t="s">
+        <v>187</v>
+      </c>
+      <c r="F70">
+        <v>3.6</v>
+      </c>
+      <c r="G70">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>221</v>
+      </c>
+      <c r="B71">
+        <v>10</v>
+      </c>
+      <c r="C71">
+        <v>207</v>
+      </c>
+      <c r="E71" t="s">
+        <v>189</v>
+      </c>
+      <c r="F71">
+        <v>5.79</v>
+      </c>
+      <c r="G71">
+        <v>5.78</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>222</v>
+      </c>
+      <c r="B72">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="C72">
+        <v>207</v>
+      </c>
+      <c r="E72" t="s">
+        <v>191</v>
+      </c>
+      <c r="F72">
+        <v>5.79</v>
+      </c>
+      <c r="G72">
+        <v>5.78</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>223</v>
+      </c>
+      <c r="B73">
+        <v>9.9</v>
+      </c>
+      <c r="C73">
+        <v>199</v>
+      </c>
+      <c r="E73" t="s">
+        <v>193</v>
+      </c>
+      <c r="F73">
+        <v>3483019</v>
+      </c>
+      <c r="G73">
+        <v>3576470</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>224</v>
+      </c>
+      <c r="B74">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="C74">
+        <v>205</v>
+      </c>
+      <c r="E74" t="s">
+        <v>195</v>
+      </c>
+      <c r="F74">
+        <v>100</v>
+      </c>
+      <c r="G74">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>225</v>
+      </c>
+      <c r="B75">
+        <v>10</v>
+      </c>
+      <c r="C75">
+        <v>214</v>
+      </c>
+      <c r="E75" t="s">
+        <v>197</v>
+      </c>
+      <c r="F75">
+        <v>1901603</v>
+      </c>
+      <c r="G75">
+        <v>2086918</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>226</v>
+      </c>
+      <c r="B76">
+        <v>12</v>
+      </c>
+      <c r="C76">
+        <v>216</v>
+      </c>
+      <c r="E76" t="s">
+        <v>199</v>
+      </c>
+      <c r="F76">
+        <v>63.3</v>
+      </c>
+      <c r="G76">
+        <v>65.400000000000006</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>227</v>
+      </c>
+      <c r="B77">
+        <v>12.4</v>
+      </c>
+      <c r="C77">
+        <v>220</v>
+      </c>
+      <c r="E77" t="s">
+        <v>201</v>
+      </c>
+      <c r="F77">
+        <v>4704</v>
+      </c>
+      <c r="G77">
+        <v>3728</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>228</v>
+      </c>
+      <c r="B78">
+        <v>11.8</v>
+      </c>
+      <c r="C78">
+        <v>191</v>
+      </c>
+      <c r="E78" t="s">
+        <v>203</v>
+      </c>
+      <c r="F78">
+        <v>1821</v>
+      </c>
+      <c r="G78">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>229</v>
+      </c>
+      <c r="B79">
+        <v>11</v>
+      </c>
+      <c r="C79">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>230</v>
+      </c>
+      <c r="B80">
+        <v>10.4</v>
+      </c>
+      <c r="C80">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>231</v>
+      </c>
+      <c r="B81">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="C81">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>232</v>
+      </c>
+      <c r="B82">
+        <v>10.6</v>
+      </c>
+      <c r="C82">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>233</v>
+      </c>
+      <c r="B83">
+        <v>9.4</v>
+      </c>
+      <c r="C83">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>234</v>
+      </c>
+      <c r="B84">
+        <v>9</v>
+      </c>
+      <c r="C84">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>235</v>
+      </c>
+      <c r="B85">
+        <v>8.1</v>
+      </c>
+      <c r="C85">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>236</v>
+      </c>
+      <c r="B86">
+        <v>9.4</v>
+      </c>
+      <c r="C86">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>237</v>
+      </c>
+      <c r="B87">
+        <v>8.5</v>
+      </c>
+      <c r="C87">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>238</v>
+      </c>
+      <c r="B88">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C88">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>239</v>
+      </c>
+      <c r="B89">
+        <v>7.9</v>
+      </c>
+      <c r="C89">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>240</v>
+      </c>
+      <c r="B90">
+        <v>8.9</v>
+      </c>
+      <c r="C90">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>241</v>
+      </c>
+      <c r="B91">
+        <v>9.6</v>
+      </c>
+      <c r="C91">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>242</v>
+      </c>
+      <c r="B92">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="C92">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>243</v>
+      </c>
+      <c r="B93">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="C93">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>244</v>
+      </c>
+      <c r="B94">
+        <v>8.6</v>
+      </c>
+      <c r="C94">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>245</v>
+      </c>
+      <c r="B95">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="C95">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>246</v>
+      </c>
+      <c r="B96">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C96">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>247</v>
+      </c>
+      <c r="B97">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C97">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>248</v>
+      </c>
+      <c r="B98">
+        <v>7.9</v>
+      </c>
+      <c r="C98">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>249</v>
+      </c>
+      <c r="B99">
+        <v>8.6</v>
+      </c>
+      <c r="C99">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>250</v>
+      </c>
+      <c r="B100">
+        <v>8.4</v>
+      </c>
+      <c r="C100">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>251</v>
+      </c>
+      <c r="B101">
+        <v>8.1</v>
+      </c>
+      <c r="C101">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>252</v>
+      </c>
+      <c r="B102">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C102">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>253</v>
+      </c>
+      <c r="B103">
+        <v>6.9</v>
+      </c>
+      <c r="C103">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>254</v>
+      </c>
+      <c r="B104">
+        <v>6.5</v>
+      </c>
+      <c r="C104">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>255</v>
+      </c>
+      <c r="B105">
+        <v>7.7</v>
+      </c>
+      <c r="C105">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>256</v>
+      </c>
+      <c r="B106">
+        <v>6.1</v>
+      </c>
+      <c r="C106">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>257</v>
+      </c>
+      <c r="B107">
+        <v>6.2</v>
+      </c>
+      <c r="C107">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>258</v>
+      </c>
+      <c r="B108">
+        <v>6.5</v>
+      </c>
+      <c r="C108">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>259</v>
+      </c>
+      <c r="B109">
+        <v>5.4</v>
+      </c>
+      <c r="C109">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>260</v>
+      </c>
+      <c r="B110">
+        <v>8</v>
+      </c>
+      <c r="C110">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>261</v>
+      </c>
+      <c r="B111">
+        <v>6.6</v>
+      </c>
+      <c r="C111">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>262</v>
+      </c>
+      <c r="B112">
+        <v>6.7</v>
+      </c>
+      <c r="C112">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>263</v>
+      </c>
+      <c r="B113">
+        <v>7.2</v>
+      </c>
+      <c r="C113">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>264</v>
+      </c>
+      <c r="B114">
+        <v>7.6</v>
+      </c>
+      <c r="C114">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>265</v>
+      </c>
+      <c r="B115">
+        <v>6.3</v>
+      </c>
+      <c r="C115">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>266</v>
+      </c>
+      <c r="B116">
+        <v>6.2</v>
+      </c>
+      <c r="C116">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>211</v>
+      </c>
+      <c r="B119">
+        <v>10</v>
+      </c>
+      <c r="C119">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>212</v>
+      </c>
+      <c r="B120">
+        <v>10.3</v>
+      </c>
+      <c r="C120">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>213</v>
+      </c>
+      <c r="B121">
+        <v>12.7</v>
+      </c>
+      <c r="C121">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>214</v>
+      </c>
+      <c r="B122">
+        <v>11.4</v>
+      </c>
+      <c r="C122">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>215</v>
+      </c>
+      <c r="B123">
+        <v>11.1</v>
+      </c>
+      <c r="C123">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>216</v>
+      </c>
+      <c r="B124">
+        <v>10</v>
+      </c>
+      <c r="C124">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>217</v>
+      </c>
+      <c r="B125">
+        <v>9.4</v>
+      </c>
+      <c r="C125">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>218</v>
+      </c>
+      <c r="B126">
+        <v>10.7</v>
+      </c>
+      <c r="C126">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>219</v>
+      </c>
+      <c r="B127">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C127">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>220</v>
+      </c>
+      <c r="B128">
+        <v>10.6</v>
+      </c>
+      <c r="C128">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>221</v>
+      </c>
+      <c r="B129">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="C129">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>222</v>
+      </c>
+      <c r="B130">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="C130">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>223</v>
+      </c>
+      <c r="B131">
+        <v>9.4</v>
+      </c>
+      <c r="C131">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>224</v>
+      </c>
+      <c r="B132">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="C132">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>225</v>
+      </c>
+      <c r="B133">
+        <v>12.6</v>
+      </c>
+      <c r="C133">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>226</v>
+      </c>
+      <c r="B134">
+        <v>10.3</v>
+      </c>
+      <c r="C134">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>227</v>
+      </c>
+      <c r="B135">
+        <v>10.1</v>
+      </c>
+      <c r="C135">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>228</v>
+      </c>
+      <c r="B136">
+        <v>10.9</v>
+      </c>
+      <c r="C136">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>229</v>
+      </c>
+      <c r="B137">
+        <v>11.3</v>
+      </c>
+      <c r="C137">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>230</v>
+      </c>
+      <c r="B138">
+        <v>11.6</v>
+      </c>
+      <c r="C138">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>231</v>
+      </c>
+      <c r="B139">
+        <v>10.5</v>
+      </c>
+      <c r="C139">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>232</v>
+      </c>
+      <c r="B140">
+        <v>10.5</v>
+      </c>
+      <c r="C140">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>233</v>
+      </c>
+      <c r="B141">
+        <v>10.3</v>
+      </c>
+      <c r="C141">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>234</v>
+      </c>
+      <c r="B142">
+        <v>10.9</v>
+      </c>
+      <c r="C142">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>235</v>
+      </c>
+      <c r="B143">
+        <v>9</v>
+      </c>
+      <c r="C143">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>236</v>
+      </c>
+      <c r="B144">
+        <v>12</v>
+      </c>
+      <c r="C144">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>237</v>
+      </c>
+      <c r="B145">
+        <v>11.8</v>
+      </c>
+      <c r="C145">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>238</v>
+      </c>
+      <c r="B146">
+        <v>12.7</v>
+      </c>
+      <c r="C146">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>239</v>
+      </c>
+      <c r="B147">
+        <v>12.5</v>
+      </c>
+      <c r="C147">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>240</v>
+      </c>
+      <c r="B148">
+        <v>13.1</v>
+      </c>
+      <c r="C148">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>241</v>
+      </c>
+      <c r="B149">
+        <v>11.2</v>
+      </c>
+      <c r="C149">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>242</v>
+      </c>
+      <c r="B150">
+        <v>12.2</v>
+      </c>
+      <c r="C150">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>243</v>
+      </c>
+      <c r="B151">
+        <v>12</v>
+      </c>
+      <c r="C151">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>244</v>
+      </c>
+      <c r="B152">
+        <v>13.4</v>
+      </c>
+      <c r="C152">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>245</v>
+      </c>
+      <c r="B153">
+        <v>12.5</v>
+      </c>
+      <c r="C153">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>246</v>
+      </c>
+      <c r="B154">
+        <v>12.6</v>
+      </c>
+      <c r="C154">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>247</v>
+      </c>
+      <c r="B155">
+        <v>13.1</v>
+      </c>
+      <c r="C155">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>248</v>
+      </c>
+      <c r="B156">
+        <v>13.3</v>
+      </c>
+      <c r="C156">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>249</v>
+      </c>
+      <c r="B157">
+        <v>13.9</v>
+      </c>
+      <c r="C157">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>250</v>
+      </c>
+      <c r="B158">
+        <v>13</v>
+      </c>
+      <c r="C158">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>251</v>
+      </c>
+      <c r="B159">
+        <v>14.3</v>
+      </c>
+      <c r="C159">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>252</v>
+      </c>
+      <c r="B160">
+        <v>10.7</v>
+      </c>
+      <c r="C160">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>253</v>
+      </c>
+      <c r="B161">
+        <v>10.6</v>
+      </c>
+      <c r="C161">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>254</v>
+      </c>
+      <c r="B162">
+        <v>12</v>
+      </c>
+      <c r="C162">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>255</v>
+      </c>
+      <c r="B163">
+        <v>12.6</v>
+      </c>
+      <c r="C163">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>256</v>
+      </c>
+      <c r="B164">
+        <v>12.7</v>
+      </c>
+      <c r="C164">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>257</v>
+      </c>
+      <c r="B165">
+        <v>13.6</v>
+      </c>
+      <c r="C165">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>258</v>
+      </c>
+      <c r="B166">
+        <v>10.9</v>
+      </c>
+      <c r="C166">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>259</v>
+      </c>
+      <c r="B167">
+        <v>11.9</v>
+      </c>
+      <c r="C167">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>260</v>
+      </c>
+      <c r="B168">
+        <v>11.1</v>
+      </c>
+      <c r="C168">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>261</v>
+      </c>
+      <c r="B169">
+        <v>13.3</v>
+      </c>
+      <c r="C169">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>262</v>
+      </c>
+      <c r="B170">
+        <v>10.8</v>
+      </c>
+      <c r="C170">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>263</v>
+      </c>
+      <c r="B171">
+        <v>11.2</v>
+      </c>
+      <c r="C171">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>264</v>
+      </c>
+      <c r="B172">
+        <v>12.1</v>
+      </c>
+      <c r="C172">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>265</v>
+      </c>
+      <c r="B173">
+        <v>11.7</v>
+      </c>
+      <c r="C173">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>266</v>
+      </c>
+      <c r="B174">
+        <v>12.3</v>
+      </c>
+      <c r="C174">
+        <v>350</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C25"/>

</xml_diff>

<commit_message>
Complementacion del archivo de entrada principal
</commit_message>
<xml_diff>
--- a/Plantilla_Entrada_5W1H.xlsx
+++ b/Plantilla_Entrada_5W1H.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NavaG\Downloads\5W1H\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22486E58-B2C3-40B0-ABFE-BBA91A767CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A814D3-3145-44D5-964F-5A5F2C345CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="949" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -1017,7 +1017,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="281">
   <si>
     <t>Plantilla de Entrada 5W1H</t>
   </si>
@@ -1175,9 +1175,6 @@
     <t>  - `6`: Competencia.</t>
   </si>
   <si>
-    <t>- Asegurese de que la primera hoja comience con `1_` porque el script usa esa pestana para obtener la marca que se mostrara en el nombre del archivo final.</t>
-  </si>
-  <si>
     <t>Nombres y estructura de las hojas (pestañas)</t>
   </si>
   <si>
@@ -1196,12 +1193,6 @@
     <t>  - `6-1`: Competencia, Precio Indexado</t>
   </si>
   <si>
-    <t>U/L/K/T/R/M</t>
-  </si>
-  <si>
-    <t>  - `2-Unidad`: Por que? (arbol - datos MAT).</t>
-  </si>
-  <si>
     <t>NOMENCOL = Cp - Palmolive\Total NOMENCOL</t>
   </si>
   <si>
@@ -1818,13 +1809,64 @@
   </si>
   <si>
     <t xml:space="preserve">    Aug-25  </t>
+  </si>
+  <si>
+    <t>EJEMPLO</t>
+  </si>
+  <si>
+    <t>1_Coca Cola</t>
+  </si>
+  <si>
+    <t>4_Coca Cola</t>
+  </si>
+  <si>
+    <t>3_Coca Cola_1</t>
+  </si>
+  <si>
+    <t>3_Coca Cola_3</t>
+  </si>
+  <si>
+    <t>5_Coca Cola_1</t>
+  </si>
+  <si>
+    <t>5_Coca Cola_2</t>
+  </si>
+  <si>
+    <t>6_Coca Cola_1</t>
+  </si>
+  <si>
+    <t>3_Coca Cola_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6_Gaseosas </t>
+  </si>
+  <si>
+    <t>7_Gaseosas</t>
+  </si>
+  <si>
+    <t>8_Gaseosas</t>
+  </si>
+  <si>
+    <t>2_Coca Cola_L</t>
+  </si>
+  <si>
+    <t>Valores extras</t>
+  </si>
+  <si>
+    <t>Asegurese de que la primera hoja comience con el numero de la pregunta `1_` porque el script usa esa pestana para obtener la marca que se mostrara en el nombre del archivo final.</t>
+  </si>
+  <si>
+    <t>  - `2-Unidad`: Por que? (Arbol de Medidas - MAT).</t>
+  </si>
+  <si>
+    <t>U/L/K/T/R/M/H</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1866,8 +1908,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1911,6 +1960,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1933,7 +1994,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1972,7 +2033,8 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2368,17 +2430,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
+      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="80" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="1" max="1" width="77.140625" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
@@ -2461,105 +2524,147 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="21" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B26" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="C27" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="B28" t="s">
+        <v>280</v>
+      </c>
+      <c r="C28" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="C29" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="C30" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="C31" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="C32" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="C33" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="C34" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="20" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>98</v>
-      </c>
-      <c r="B36" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>52</v>
+      <c r="C35" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="17" t="s">
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -3032,7 +3137,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>38</v>
@@ -3545,31 +3650,31 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" t="s">
         <v>90</v>
-      </c>
-      <c r="B3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B4">
         <v>100</v>
@@ -3583,7 +3688,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B5">
         <v>74.599999999999994</v>
@@ -3597,7 +3702,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B6">
         <v>24.3</v>
@@ -3611,7 +3716,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B7">
         <v>1.1000000000000001</v>
@@ -3632,7 +3737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A3A67E-8AC6-4000-96DE-0ABA21917A59}">
   <dimension ref="A1:G174"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -3640,36 +3745,36 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D1" s="19"/>
       <c r="E1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B3">
         <v>52.5</v>
@@ -3678,7 +3783,7 @@
         <v>973</v>
       </c>
       <c r="E3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F3">
         <v>10944760</v>
@@ -3689,7 +3794,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B4">
         <v>51.1</v>
@@ -3698,7 +3803,7 @@
         <v>961</v>
       </c>
       <c r="E4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F4">
         <v>100</v>
@@ -3709,7 +3814,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B5">
         <v>52.6</v>
@@ -3718,7 +3823,7 @@
         <v>998</v>
       </c>
       <c r="E5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F5">
         <v>10945</v>
@@ -3729,7 +3834,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B6">
         <v>52.9</v>
@@ -3738,7 +3843,7 @@
         <v>988</v>
       </c>
       <c r="E6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F6">
         <v>48240360</v>
@@ -3749,7 +3854,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B7">
         <v>53.6</v>
@@ -3758,7 +3863,7 @@
         <v>1042</v>
       </c>
       <c r="E7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F7">
         <v>100</v>
@@ -3769,7 +3874,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B8">
         <v>51.5</v>
@@ -3778,7 +3883,7 @@
         <v>958</v>
       </c>
       <c r="E8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F8">
         <v>48240360</v>
@@ -3789,7 +3894,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B9">
         <v>50.7</v>
@@ -3798,7 +3903,7 @@
         <v>957</v>
       </c>
       <c r="E9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F9">
         <v>100</v>
@@ -3809,7 +3914,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B10">
         <v>48.5</v>
@@ -3818,7 +3923,7 @@
         <v>921</v>
       </c>
       <c r="E10" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F10">
         <v>86.3</v>
@@ -3829,7 +3934,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B11">
         <v>45.2</v>
@@ -3837,8 +3942,8 @@
       <c r="C11">
         <v>846</v>
       </c>
-      <c r="E11" s="20" t="s">
-        <v>122</v>
+      <c r="E11" t="s">
+        <v>119</v>
       </c>
       <c r="F11">
         <v>100</v>
@@ -3849,7 +3954,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B12">
         <v>50.5</v>
@@ -3858,7 +3963,7 @@
         <v>926</v>
       </c>
       <c r="E12" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F12">
         <v>3.64</v>
@@ -3869,7 +3974,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B13">
         <v>48.1</v>
@@ -3878,7 +3983,7 @@
         <v>858</v>
       </c>
       <c r="E13" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F13">
         <v>16.059999999999999</v>
@@ -3889,7 +3994,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B14">
         <v>51.6</v>
@@ -3898,7 +4003,7 @@
         <v>941</v>
       </c>
       <c r="E14" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F14">
         <v>16.059999999999999</v>
@@ -3909,7 +4014,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B15">
         <v>51.1</v>
@@ -3918,7 +4023,7 @@
         <v>923</v>
       </c>
       <c r="E15" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F15">
         <v>0.5</v>
@@ -3929,7 +4034,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B16">
         <v>48.6</v>
@@ -3938,7 +4043,7 @@
         <v>891</v>
       </c>
       <c r="E16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F16">
         <v>2.2000000000000002</v>
@@ -3949,7 +4054,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B17">
         <v>53.5</v>
@@ -3958,7 +4063,7 @@
         <v>958</v>
       </c>
       <c r="E17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F17">
         <v>2.2000000000000002</v>
@@ -3969,7 +4074,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B18">
         <v>48.2</v>
@@ -3978,7 +4083,7 @@
         <v>856</v>
       </c>
       <c r="E18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F18">
         <v>7.3</v>
@@ -3989,7 +4094,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B19">
         <v>48.2</v>
@@ -3998,7 +4103,7 @@
         <v>865</v>
       </c>
       <c r="E19" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F19">
         <v>4.7300000000000004</v>
@@ -4009,7 +4114,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B20">
         <v>45.8</v>
@@ -4018,7 +4123,7 @@
         <v>814</v>
       </c>
       <c r="E20" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F20">
         <v>4.7300000000000004</v>
@@ -4029,7 +4134,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B21">
         <v>44.1</v>
@@ -4038,7 +4143,7 @@
         <v>809</v>
       </c>
       <c r="E21" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F21">
         <v>3483019</v>
@@ -4049,7 +4154,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B22">
         <v>42.7</v>
@@ -4058,7 +4163,7 @@
         <v>774</v>
       </c>
       <c r="E22" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F22">
         <v>100</v>
@@ -4069,7 +4174,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B23">
         <v>41.4</v>
@@ -4078,7 +4183,7 @@
         <v>746</v>
       </c>
       <c r="E23" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F23">
         <v>3004475</v>
@@ -4089,7 +4194,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B24">
         <v>42.5</v>
@@ -4098,7 +4203,7 @@
         <v>766</v>
       </c>
       <c r="E24" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F24">
         <v>100</v>
@@ -4109,7 +4214,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B25">
         <v>42.9</v>
@@ -4118,7 +4223,7 @@
         <v>753</v>
       </c>
       <c r="E25" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F25">
         <v>4704</v>
@@ -4129,7 +4234,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B26">
         <v>41.1</v>
@@ -4138,7 +4243,7 @@
         <v>743</v>
       </c>
       <c r="E26" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F26">
         <v>3253</v>
@@ -4149,7 +4254,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B27">
         <v>37.4</v>
@@ -4160,7 +4265,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B28">
         <v>39.5</v>
@@ -4169,12 +4274,12 @@
         <v>689</v>
       </c>
       <c r="E28" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B29">
         <v>40.6</v>
@@ -4183,7 +4288,7 @@
         <v>715</v>
       </c>
       <c r="E29" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F29">
         <v>591438</v>
@@ -4194,7 +4299,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B30">
         <v>38.700000000000003</v>
@@ -4203,7 +4308,7 @@
         <v>673</v>
       </c>
       <c r="E30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F30">
         <v>5.4</v>
@@ -4214,7 +4319,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B31">
         <v>39.700000000000003</v>
@@ -4223,7 +4328,7 @@
         <v>719</v>
       </c>
       <c r="E31" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F31">
         <v>591</v>
@@ -4234,7 +4339,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B32">
         <v>40.1</v>
@@ -4243,7 +4348,7 @@
         <v>665</v>
       </c>
       <c r="E32" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F32">
         <v>5927047</v>
@@ -4254,7 +4359,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B33">
         <v>38.700000000000003</v>
@@ -4263,7 +4368,7 @@
         <v>1014</v>
       </c>
       <c r="E33" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F33">
         <v>12.3</v>
@@ -4274,7 +4379,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B34">
         <v>36.200000000000003</v>
@@ -4283,7 +4388,7 @@
         <v>947</v>
       </c>
       <c r="E34" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F34">
         <v>5927047</v>
@@ -4294,7 +4399,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B35">
         <v>36.299999999999997</v>
@@ -4303,7 +4408,7 @@
         <v>1013</v>
       </c>
       <c r="E35" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F35">
         <v>12.3</v>
@@ -4314,7 +4419,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B36">
         <v>37.1</v>
@@ -4323,7 +4428,7 @@
         <v>959</v>
       </c>
       <c r="E36" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F36">
         <v>34.799999999999997</v>
@@ -4334,7 +4439,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B37">
         <v>37.1</v>
@@ -4343,7 +4448,7 @@
         <v>966</v>
       </c>
       <c r="E37" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F37">
         <v>40.4</v>
@@ -4354,7 +4459,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B38">
         <v>36.6</v>
@@ -4363,7 +4468,7 @@
         <v>987</v>
       </c>
       <c r="E38" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F38">
         <v>0.49</v>
@@ -4374,7 +4479,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B39">
         <v>38.1</v>
@@ -4383,7 +4488,7 @@
         <v>967</v>
       </c>
       <c r="E39" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F39">
         <v>4.88</v>
@@ -4394,7 +4499,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B40">
         <v>35.700000000000003</v>
@@ -4403,7 +4508,7 @@
         <v>927</v>
       </c>
       <c r="E40" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F40">
         <v>4.88</v>
@@ -4414,7 +4519,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B41">
         <v>36.5</v>
@@ -4423,7 +4528,7 @@
         <v>969</v>
       </c>
       <c r="E41" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F41">
         <v>0.16</v>
@@ -4434,7 +4539,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B42">
         <v>35.799999999999997</v>
@@ -4443,7 +4548,7 @@
         <v>940</v>
       </c>
       <c r="E42" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F42">
         <v>1.61</v>
@@ -4454,7 +4559,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B43">
         <v>35.299999999999997</v>
@@ -4463,7 +4568,7 @@
         <v>1056</v>
       </c>
       <c r="E43" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F43">
         <v>1.61</v>
@@ -4474,7 +4579,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B44">
         <v>33.700000000000003</v>
@@ -4483,7 +4588,7 @@
         <v>1016</v>
       </c>
       <c r="E44" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F44">
         <v>3</v>
@@ -4494,7 +4599,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B45">
         <v>31.6</v>
@@ -4503,7 +4608,7 @@
         <v>910</v>
       </c>
       <c r="E45" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F45">
         <v>11.18</v>
@@ -4514,7 +4619,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B46">
         <v>32.5</v>
@@ -4523,7 +4628,7 @@
         <v>883</v>
       </c>
       <c r="E46" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F46">
         <v>11.18</v>
@@ -4534,7 +4639,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B47">
         <v>34.299999999999997</v>
@@ -4543,7 +4648,7 @@
         <v>943</v>
       </c>
       <c r="E47" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F47">
         <v>3483019</v>
@@ -4554,7 +4659,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B48">
         <v>32</v>
@@ -4563,7 +4668,7 @@
         <v>918</v>
       </c>
       <c r="E48" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F48">
         <v>100</v>
@@ -4574,7 +4679,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B49">
         <v>34</v>
@@ -4583,7 +4688,7 @@
         <v>900</v>
       </c>
       <c r="E49" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F49">
         <v>1213634</v>
@@ -4594,7 +4699,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B50">
         <v>30.3</v>
@@ -4603,7 +4708,7 @@
         <v>886</v>
       </c>
       <c r="E50" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F50">
         <v>40.4</v>
@@ -4614,7 +4719,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B51">
         <v>32.200000000000003</v>
@@ -4623,7 +4728,7 @@
         <v>920</v>
       </c>
       <c r="E51" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F51">
         <v>4704</v>
@@ -4634,7 +4739,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B52">
         <v>32.299999999999997</v>
@@ -4643,7 +4748,7 @@
         <v>965</v>
       </c>
       <c r="E52" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F52">
         <v>1132</v>
@@ -4654,7 +4759,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B53">
         <v>35.9</v>
@@ -4665,7 +4770,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B54">
         <v>33.200000000000003</v>
@@ -4674,12 +4779,12 @@
         <v>1001</v>
       </c>
       <c r="E54" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B55">
         <v>33.200000000000003</v>
@@ -4688,7 +4793,7 @@
         <v>1012</v>
       </c>
       <c r="E55" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F55">
         <v>2842228</v>
@@ -4699,7 +4804,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B56">
         <v>34.9</v>
@@ -4708,7 +4813,7 @@
         <v>975</v>
       </c>
       <c r="E56" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F56">
         <v>26</v>
@@ -4719,7 +4824,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B57">
         <v>31.7</v>
@@ -4728,7 +4833,7 @@
         <v>1006</v>
       </c>
       <c r="E57" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F57">
         <v>2842</v>
@@ -4739,7 +4844,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B58">
         <v>35.5</v>
@@ -4748,7 +4853,7 @@
         <v>999</v>
       </c>
       <c r="E58" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F58">
         <v>15197020</v>
@@ -4759,7 +4864,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E59" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F59">
         <v>31.5</v>
@@ -4770,10 +4875,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E60" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F60">
         <v>15197020</v>
@@ -4784,7 +4889,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B61">
         <v>11.2</v>
@@ -4793,7 +4898,7 @@
         <v>274</v>
       </c>
       <c r="E61" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F61">
         <v>31.5</v>
@@ -4804,7 +4909,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B62">
         <v>12.2</v>
@@ -4813,7 +4918,7 @@
         <v>274</v>
       </c>
       <c r="E62" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F62">
         <v>54.6</v>
@@ -4824,7 +4929,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B63">
         <v>13.2</v>
@@ -4833,7 +4938,7 @@
         <v>302</v>
       </c>
       <c r="E63" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F63">
         <v>63.3</v>
@@ -4844,7 +4949,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B64">
         <v>12</v>
@@ -4853,7 +4958,7 @@
         <v>305</v>
       </c>
       <c r="E64" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F64">
         <v>1.49</v>
@@ -4864,7 +4969,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B65">
         <v>12.3</v>
@@ -4873,7 +4978,7 @@
         <v>300</v>
       </c>
       <c r="E65" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F65">
         <v>7.99</v>
@@ -4884,7 +4989,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B66">
         <v>10.4</v>
@@ -4893,7 +4998,7 @@
         <v>247</v>
       </c>
       <c r="E66" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F66">
         <v>7.99</v>
@@ -4904,7 +5009,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B67">
         <v>10.1</v>
@@ -4913,7 +5018,7 @@
         <v>256</v>
       </c>
       <c r="E67" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F67">
         <v>0.42</v>
@@ -4924,7 +5029,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B68">
         <v>10.6</v>
@@ -4933,7 +5038,7 @@
         <v>242</v>
       </c>
       <c r="E68" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F68">
         <v>2.25</v>
@@ -4944,7 +5049,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B69">
         <v>9.8000000000000007</v>
@@ -4953,7 +5058,7 @@
         <v>222</v>
       </c>
       <c r="E69" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F69">
         <v>2.25</v>
@@ -4964,7 +5069,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B70">
         <v>11.5</v>
@@ -4973,7 +5078,7 @@
         <v>249</v>
       </c>
       <c r="E70" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F70">
         <v>3.6</v>
@@ -4984,7 +5089,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B71">
         <v>10</v>
@@ -4993,7 +5098,7 @@
         <v>207</v>
       </c>
       <c r="E71" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F71">
         <v>5.79</v>
@@ -5004,7 +5109,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B72">
         <v>9.6999999999999993</v>
@@ -5013,7 +5118,7 @@
         <v>207</v>
       </c>
       <c r="E72" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F72">
         <v>5.79</v>
@@ -5024,7 +5129,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B73">
         <v>9.9</v>
@@ -5033,7 +5138,7 @@
         <v>199</v>
       </c>
       <c r="E73" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F73">
         <v>3483019</v>
@@ -5044,7 +5149,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B74">
         <v>9.8000000000000007</v>
@@ -5053,7 +5158,7 @@
         <v>205</v>
       </c>
       <c r="E74" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F74">
         <v>100</v>
@@ -5064,7 +5169,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B75">
         <v>10</v>
@@ -5073,7 +5178,7 @@
         <v>214</v>
       </c>
       <c r="E75" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F75">
         <v>1901603</v>
@@ -5084,7 +5189,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B76">
         <v>12</v>
@@ -5093,7 +5198,7 @@
         <v>216</v>
       </c>
       <c r="E76" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F76">
         <v>63.3</v>
@@ -5104,7 +5209,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B77">
         <v>12.4</v>
@@ -5113,7 +5218,7 @@
         <v>220</v>
       </c>
       <c r="E77" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F77">
         <v>4704</v>
@@ -5124,7 +5229,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B78">
         <v>11.8</v>
@@ -5133,7 +5238,7 @@
         <v>191</v>
       </c>
       <c r="E78" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F78">
         <v>1821</v>
@@ -5144,7 +5249,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B79">
         <v>11</v>
@@ -5155,7 +5260,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B80">
         <v>10.4</v>
@@ -5166,7 +5271,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B81">
         <v>9.6999999999999993</v>
@@ -5177,7 +5282,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B82">
         <v>10.6</v>
@@ -5188,7 +5293,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B83">
         <v>9.4</v>
@@ -5199,7 +5304,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B84">
         <v>9</v>
@@ -5210,7 +5315,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B85">
         <v>8.1</v>
@@ -5221,7 +5326,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B86">
         <v>9.4</v>
@@ -5232,7 +5337,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B87">
         <v>8.5</v>
@@ -5243,7 +5348,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B88">
         <v>8.1999999999999993</v>
@@ -5254,7 +5359,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B89">
         <v>7.9</v>
@@ -5265,7 +5370,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B90">
         <v>8.9</v>
@@ -5276,7 +5381,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B91">
         <v>9.6</v>
@@ -5287,7 +5392,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B92">
         <v>9.3000000000000007</v>
@@ -5298,7 +5403,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B93">
         <v>8.6999999999999993</v>
@@ -5309,7 +5414,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B94">
         <v>8.6</v>
@@ -5320,7 +5425,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B95">
         <v>8.3000000000000007</v>
@@ -5331,7 +5436,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B96">
         <v>8.1999999999999993</v>
@@ -5342,7 +5447,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B97">
         <v>8.1999999999999993</v>
@@ -5353,7 +5458,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B98">
         <v>7.9</v>
@@ -5364,7 +5469,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B99">
         <v>8.6</v>
@@ -5375,7 +5480,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B100">
         <v>8.4</v>
@@ -5386,7 +5491,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B101">
         <v>8.1</v>
@@ -5397,7 +5502,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B102">
         <v>8.1999999999999993</v>
@@ -5408,7 +5513,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B103">
         <v>6.9</v>
@@ -5419,7 +5524,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B104">
         <v>6.5</v>
@@ -5430,7 +5535,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B105">
         <v>7.7</v>
@@ -5441,7 +5546,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B106">
         <v>6.1</v>
@@ -5452,7 +5557,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B107">
         <v>6.2</v>
@@ -5463,7 +5568,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B108">
         <v>6.5</v>
@@ -5474,7 +5579,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B109">
         <v>5.4</v>
@@ -5485,7 +5590,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B110">
         <v>8</v>
@@ -5496,7 +5601,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B111">
         <v>6.6</v>
@@ -5507,7 +5612,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B112">
         <v>6.7</v>
@@ -5518,7 +5623,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B113">
         <v>7.2</v>
@@ -5529,7 +5634,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B114">
         <v>7.6</v>
@@ -5540,7 +5645,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B115">
         <v>6.3</v>
@@ -5551,7 +5656,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B116">
         <v>6.2</v>
@@ -5562,12 +5667,12 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B119">
         <v>10</v>
@@ -5578,7 +5683,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B120">
         <v>10.3</v>
@@ -5589,7 +5694,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B121">
         <v>12.7</v>
@@ -5600,7 +5705,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B122">
         <v>11.4</v>
@@ -5611,7 +5716,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B123">
         <v>11.1</v>
@@ -5622,7 +5727,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B124">
         <v>10</v>
@@ -5633,7 +5738,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B125">
         <v>9.4</v>
@@ -5644,7 +5749,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B126">
         <v>10.7</v>
@@ -5655,7 +5760,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B127">
         <v>8.1999999999999993</v>
@@ -5666,7 +5771,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B128">
         <v>10.6</v>
@@ -5677,7 +5782,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B129">
         <v>9.8000000000000007</v>
@@ -5688,7 +5793,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B130">
         <v>9.6999999999999993</v>
@@ -5699,7 +5804,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B131">
         <v>9.4</v>
@@ -5710,7 +5815,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B132">
         <v>9.8000000000000007</v>
@@ -5721,7 +5826,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B133">
         <v>12.6</v>
@@ -5732,7 +5837,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B134">
         <v>10.3</v>
@@ -5743,7 +5848,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B135">
         <v>10.1</v>
@@ -5754,7 +5859,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B136">
         <v>10.9</v>
@@ -5765,7 +5870,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B137">
         <v>11.3</v>
@@ -5776,7 +5881,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B138">
         <v>11.6</v>
@@ -5787,7 +5892,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B139">
         <v>10.5</v>
@@ -5798,7 +5903,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B140">
         <v>10.5</v>
@@ -5809,7 +5914,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B141">
         <v>10.3</v>
@@ -5820,7 +5925,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B142">
         <v>10.9</v>
@@ -5831,7 +5936,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B143">
         <v>9</v>
@@ -5842,7 +5947,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B144">
         <v>12</v>
@@ -5853,7 +5958,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B145">
         <v>11.8</v>
@@ -5864,7 +5969,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B146">
         <v>12.7</v>
@@ -5875,7 +5980,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B147">
         <v>12.5</v>
@@ -5886,7 +5991,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B148">
         <v>13.1</v>
@@ -5897,7 +6002,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B149">
         <v>11.2</v>
@@ -5908,7 +6013,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B150">
         <v>12.2</v>
@@ -5919,7 +6024,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B151">
         <v>12</v>
@@ -5930,7 +6035,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B152">
         <v>13.4</v>
@@ -5941,7 +6046,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B153">
         <v>12.5</v>
@@ -5952,7 +6057,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B154">
         <v>12.6</v>
@@ -5963,7 +6068,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B155">
         <v>13.1</v>
@@ -5974,7 +6079,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B156">
         <v>13.3</v>
@@ -5985,7 +6090,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B157">
         <v>13.9</v>
@@ -5996,7 +6101,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B158">
         <v>13</v>
@@ -6007,7 +6112,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B159">
         <v>14.3</v>
@@ -6018,7 +6123,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B160">
         <v>10.7</v>
@@ -6029,7 +6134,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B161">
         <v>10.6</v>
@@ -6040,7 +6145,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B162">
         <v>12</v>
@@ -6051,7 +6156,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B163">
         <v>12.6</v>
@@ -6062,7 +6167,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B164">
         <v>12.7</v>
@@ -6073,7 +6178,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B165">
         <v>13.6</v>
@@ -6084,7 +6189,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B166">
         <v>10.9</v>
@@ -6095,7 +6200,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B167">
         <v>11.9</v>
@@ -6106,7 +6211,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B168">
         <v>11.1</v>
@@ -6117,7 +6222,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B169">
         <v>13.3</v>
@@ -6128,7 +6233,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B170">
         <v>10.8</v>
@@ -6139,7 +6244,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B171">
         <v>11.2</v>
@@ -6150,7 +6255,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B172">
         <v>12.1</v>
@@ -6161,7 +6266,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B173">
         <v>11.7</v>
@@ -6172,7 +6277,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B174">
         <v>12.3</v>
@@ -6499,23 +6604,23 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B3">
         <v>44907</v>
@@ -6526,7 +6631,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B4">
         <v>100</v>
@@ -6537,7 +6642,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B5">
         <v>2384290</v>
@@ -6548,7 +6653,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B6">
         <v>100</v>
@@ -6559,7 +6664,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B7">
         <v>354288</v>
@@ -6570,7 +6675,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B8">
         <v>100</v>
@@ -6581,7 +6686,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B9">
         <v>7.3</v>
@@ -6592,7 +6697,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B10">
         <v>100</v>
@@ -6603,7 +6708,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B11">
         <v>0.54</v>
@@ -6614,7 +6719,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B12">
         <v>28.44</v>
@@ -6625,7 +6730,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B13">
         <v>4.2300000000000004</v>
@@ -6636,7 +6741,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B14">
         <v>0.26</v>
@@ -6647,7 +6752,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B15">
         <v>14.04</v>
@@ -6658,7 +6763,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B16">
         <v>2.09</v>
@@ -6669,7 +6774,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -6680,7 +6785,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B18">
         <v>55.96</v>
@@ -6691,7 +6796,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B19">
         <v>8.31</v>
@@ -6702,7 +6807,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B20">
         <v>1150638</v>
@@ -6713,7 +6818,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B21">
         <v>100</v>
@@ -6724,7 +6829,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B22">
         <v>83838</v>
@@ -6735,7 +6840,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B23">
         <v>100</v>
@@ -6746,7 +6851,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B24">
         <v>1134</v>
@@ -6757,7 +6862,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B25">
         <v>84</v>

</xml_diff>